<commit_message>
Changes as of 10/15
</commit_message>
<xml_diff>
--- a/InputFiles/CDS/TC02_CDS_phs002430_Sex-NotSpecified_Experimental-strategy-RNA-Seq_Filetype-fastq.xlsx
+++ b/InputFiles/CDS/TC02_CDS_phs002430_Sex-NotSpecified_Experimental-strategy-RNA-Seq_Filetype-fastq.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tatekaraa\Automation\05-29-25\Commons_Automation\InputFiles\CDS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kallakuriv2\Automation\sowjanya0909\Commons_Automation\InputFiles\CDS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCF1E208-E053-4590-8C0C-155714421296}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F29A6EC1-6717-41CA-AB1E-DCF68780767B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -55,9 +55,6 @@
   </si>
   <si>
     <t>TsvExcel</t>
-  </si>
-  <si>
-    <t>TC02_CDS_phs002430_Sex-NotSpecified_Experimental-strategy-RNA-Seq_Filetype-fastq.TSVData.xlsx</t>
   </si>
   <si>
     <t>TC02_CDS_phs002430_Sex-NotSpecified_Experimental-strategy-RNA-Seq_Filetype-fastq_WebData.xlsx</t>
@@ -222,6 +219,9 @@
     AND f.file_type = 'FASTQ'
 ORDER BY
     smp.sample_id ASC;</t>
+  </si>
+  <si>
+    <t>TC02_CDS_phs002430_Sex-NotSpecified_Experimental-strategy-RNA-Seq_Filetype-fastq_TSVData.xlsx</t>
   </si>
 </sst>
 </file>
@@ -613,19 +613,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="C2" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="75.81640625" customWidth="1"/>
-    <col min="4" max="4" width="70.1796875" customWidth="1"/>
-    <col min="5" max="5" width="87.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="75.85546875" customWidth="1"/>
+    <col min="4" max="4" width="70.140625" customWidth="1"/>
+    <col min="5" max="5" width="87.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -642,46 +642,46 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
     </row>
-    <row r="3" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4" s="2"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C6" s="1"/>
     </row>
   </sheetData>

</xml_diff>